<commit_message>
Excel Sheet connection for data
</commit_message>
<xml_diff>
--- a/POM1/ExcelData/ExcelTestData.xlsx
+++ b/POM1/ExcelData/ExcelTestData.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bassetti Training\PageObjectModel\Model1\POM1\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D971439A-C47A-476B-B11D-A814F9511312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1A8FBE2-3510-4528-BF39-7AEA64593154}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="690" yWindow="2810" windowWidth="14400" windowHeight="7270" xr2:uid="{757DFF1D-4EE8-439A-ADB7-161298B6B22E}"/>
   </bookViews>
   <sheets>
-    <sheet name="TestData1" sheetId="1" r:id="rId1"/>
+    <sheet name="LogInData" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -414,7 +414,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showFormulas="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>